<commit_message>
Cleared Test Links From Excel Files
</commit_message>
<xml_diff>
--- a/Data/Music.xlsx
+++ b/Data/Music.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\YTDownloader\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E67D75-A0CA-4E51-A534-D795DE50A80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC74676-876B-4547-9C8B-6406FB9A6EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Creators (Optional)</t>
   </si>
@@ -32,99 +32,6 @@
   </si>
   <si>
     <t>Links (Necessary)</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=pCk2jlKev64</t>
-  </si>
-  <si>
-    <t>Forever</t>
-  </si>
-  <si>
-    <t>Allie Sherlock</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=fKhdec3uyrQ</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=3QAjceoPqd0</t>
-  </si>
-  <si>
-    <t>Glimpse Of Us</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=gm9_YzsrdtQ</t>
-  </si>
-  <si>
-    <t>Easy On Me</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=FxQTY-W6GIo</t>
-  </si>
-  <si>
-    <t>Killshot</t>
-  </si>
-  <si>
-    <t>Eminem</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=o1iUYc1Y_fk</t>
-  </si>
-  <si>
-    <t>Perfect</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=rgECVKlpYq8</t>
-  </si>
-  <si>
-    <t>Until I Found You</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=KqYWi3MuUh4</t>
-  </si>
-  <si>
-    <t>Glimpse Of Us (2)</t>
-  </si>
-  <si>
-    <t>Jamal Corrie</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=w8Kw8SfEDZM</t>
-  </si>
-  <si>
-    <t>Love Story</t>
-  </si>
-  <si>
-    <t>Zoe Clarke</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=zABLecsR5UE</t>
-  </si>
-  <si>
-    <t>Someone You Loved</t>
-  </si>
-  <si>
-    <t>Lewis Capaldi</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=LEmcLFAlvEE</t>
-  </si>
-  <si>
-    <t>SOS</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=sDC2BXQNAiM</t>
-  </si>
-  <si>
-    <t>Someone You Loved (2)</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=BKc4I_cK0JU</t>
-  </si>
-  <si>
-    <t>If I Go, I'm Goin</t>
-  </si>
-  <si>
-    <t>Gregory Alan Isakov</t>
   </si>
 </sst>
 </file>
@@ -982,7 +889,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A2" sqref="A2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1008,145 +915,13 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
+      <c r="A2" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" t="s">
-        <v>34</v>
-      </c>
+      <c r="A13" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A13" r:id="rId1" xr:uid="{2FACAA2C-A5D9-480C-97F8-7087FF66E320}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>